<commit_message>
21.06.21 test_IntactFinder.py (just for RNA!!) 2
</commit_message>
<xml_diff>
--- a/Spectral_data/intact/x.xlsx
+++ b/Spectral_data/intact/x.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="51">
   <si>
     <t>parameters:</t>
   </si>
@@ -28,7 +28,7 @@
     <t>date:</t>
   </si>
   <si>
-    <t>21/06/2021 14:40</t>
+    <t>21/06/2021 15:45</t>
   </si>
   <si>
     <t>sequName</t>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>av.error:</t>
+  </si>
+  <si>
+    <t>stddev.errors:</t>
   </si>
   <si>
     <t>av. number of modifications:</t>
@@ -621,10 +624,10 @@
         <v>32</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -650,31 +653,31 @@
         <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:34">
@@ -693,9 +696,6 @@
       <c r="E19">
         <v>0.3</v>
       </c>
-      <c r="G19" t="s">
-        <v>33</v>
-      </c>
       <c r="I19">
         <v>6</v>
       </c>
@@ -703,52 +703,52 @@
         <v>0.2883430282059997</v>
       </c>
       <c r="L19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O19" t="s">
         <v>22</v>
       </c>
       <c r="P19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R19" t="s">
         <v>22</v>
       </c>
       <c r="S19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U19" t="s">
         <v>22</v>
       </c>
       <c r="V19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X19" t="s">
         <v>22</v>
       </c>
       <c r="Y19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA19" t="s">
         <v>22</v>
       </c>
       <c r="AB19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD19" t="s">
         <v>22</v>
       </c>
       <c r="AE19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG19" t="s">
         <v>22</v>
       </c>
       <c r="AH19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:34">
@@ -767,8 +767,8 @@
       <c r="E20">
         <v>0.8</v>
       </c>
-      <c r="G20" s="1">
-        <v>0.001682549762606996</v>
+      <c r="G20" t="s">
+        <v>33</v>
       </c>
       <c r="I20">
         <v>7</v>
@@ -777,7 +777,7 @@
         <v>0.2420044778973674</v>
       </c>
       <c r="L20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M20" s="2">
         <f>AVERAGE(P20:P26)</f>
@@ -842,6 +842,9 @@
       <c r="E21">
         <v>0.2</v>
       </c>
+      <c r="G21" s="1">
+        <v>0.001682549762607045</v>
+      </c>
       <c r="I21">
         <v>8</v>
       </c>
@@ -849,7 +852,7 @@
         <v>0.2160532866805435</v>
       </c>
       <c r="L21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M21" s="2">
         <f>AVERAGE(S20:S26)</f>
@@ -914,6 +917,9 @@
       <c r="E22">
         <v>0.8</v>
       </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
       <c r="I22">
         <v>9</v>
       </c>
@@ -921,7 +927,7 @@
         <v>0.2142429496101891</v>
       </c>
       <c r="L22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M22" s="2">
         <f>AVERAGE(V20:V26)</f>
@@ -986,6 +992,9 @@
       <c r="E23">
         <v>0.07000000000000001</v>
       </c>
+      <c r="G23" s="1">
+        <v>0.1248090398552634</v>
+      </c>
       <c r="I23">
         <v>10</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>0.1969289057698468</v>
       </c>
       <c r="L23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M23" s="2">
         <f>AVERAGE(Y20:Y26)</f>
@@ -1065,7 +1074,7 @@
         <v>0.1927280330419686</v>
       </c>
       <c r="L24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M24" s="2">
         <f>AVERAGE(AB20:AB26)</f>
@@ -1137,7 +1146,7 @@
         <v>0.1480257833164781</v>
       </c>
       <c r="L25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M25" s="2">
         <f>AVERAGE(AE20:AE26)</f>
@@ -1203,14 +1212,14 @@
         <v>0.11</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J26" s="1">
         <f>AVERAGE(J19:J25)</f>
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M26" s="2">
         <f>AVERAGE(AH20:AH26)</f>
@@ -1907,7 +1916,7 @@
     </row>
     <row r="66" spans="1:34">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:34">
@@ -1918,10 +1927,10 @@
         <v>32</v>
       </c>
       <c r="I67" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:34">
@@ -1947,31 +1956,31 @@
         <v>22</v>
       </c>
       <c r="J68" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O68" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA68" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD68" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG68" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:34">
@@ -1990,9 +1999,6 @@
       <c r="E69">
         <v>0.7</v>
       </c>
-      <c r="G69" t="s">
-        <v>33</v>
-      </c>
       <c r="I69">
         <v>6</v>
       </c>
@@ -2000,52 +2006,52 @@
         <v>0.3058467421416752</v>
       </c>
       <c r="L69" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O69" t="s">
         <v>22</v>
       </c>
       <c r="P69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R69" t="s">
         <v>22</v>
       </c>
       <c r="S69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U69" t="s">
         <v>22</v>
       </c>
       <c r="V69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X69" t="s">
         <v>22</v>
       </c>
       <c r="Y69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA69" t="s">
         <v>22</v>
       </c>
       <c r="AB69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD69" t="s">
         <v>22</v>
       </c>
       <c r="AE69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG69" t="s">
         <v>22</v>
       </c>
       <c r="AH69" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:34">
@@ -2064,8 +2070,8 @@
       <c r="E70">
         <v>0.51</v>
       </c>
-      <c r="G70" s="1">
-        <v>-0.01632552560005644</v>
+      <c r="G70" t="s">
+        <v>33</v>
       </c>
       <c r="I70">
         <v>7</v>
@@ -2074,7 +2080,7 @@
         <v>0.244000017611878</v>
       </c>
       <c r="L70" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M70" s="2">
         <f>AVERAGE(P70:P76)</f>
@@ -2139,6 +2145,9 @@
       <c r="E71">
         <v>1.54</v>
       </c>
+      <c r="G71" s="1">
+        <v>0.01632552560005641</v>
+      </c>
       <c r="I71">
         <v>8</v>
       </c>
@@ -2146,7 +2155,7 @@
         <v>0.2214039362926656</v>
       </c>
       <c r="L71" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M71" s="2">
         <f>AVERAGE(S70:S76)</f>
@@ -2211,6 +2220,9 @@
       <c r="E72">
         <v>0.64</v>
       </c>
+      <c r="G72" t="s">
+        <v>34</v>
+      </c>
       <c r="I72">
         <v>9</v>
       </c>
@@ -2218,7 +2230,7 @@
         <v>0.1925425061385875</v>
       </c>
       <c r="L72" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M72" s="2">
         <f>AVERAGE(V70:V76)</f>
@@ -2283,6 +2295,9 @@
       <c r="E73">
         <v>-0.22</v>
       </c>
+      <c r="G73" s="1">
+        <v>0.1823410545090352</v>
+      </c>
       <c r="I73">
         <v>10</v>
       </c>
@@ -2290,7 +2305,7 @@
         <v>0.1855150789162632</v>
       </c>
       <c r="L73" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M73" s="2">
         <f>AVERAGE(Y70:Y76)</f>
@@ -2362,7 +2377,7 @@
         <v>0.193393580483101</v>
       </c>
       <c r="L74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M74" s="2">
         <f>AVERAGE(AB70:AB76)</f>
@@ -2434,7 +2449,7 @@
         <v>0.166940412656703</v>
       </c>
       <c r="L75" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M75" s="2">
         <f>AVERAGE(AE70:AE76)</f>
@@ -2500,14 +2515,14 @@
         <v>0.34</v>
       </c>
       <c r="I76" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J76" s="1">
         <f>AVERAGE(J69:J75)</f>
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M76" s="2">
         <f>AVERAGE(AH70:AH76)</f>
@@ -3204,7 +3219,7 @@
     </row>
     <row r="116" spans="1:34">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:34">
@@ -3215,10 +3230,10 @@
         <v>32</v>
       </c>
       <c r="I117" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L117" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:34">
@@ -3244,31 +3259,31 @@
         <v>22</v>
       </c>
       <c r="J118" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L118" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O118" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R118" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U118" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X118" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA118" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD118" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG118" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:34">
@@ -3287,9 +3302,6 @@
       <c r="E119">
         <v>1.11</v>
       </c>
-      <c r="G119" t="s">
-        <v>33</v>
-      </c>
       <c r="I119">
         <v>6</v>
       </c>
@@ -3297,52 +3309,52 @@
         <v>0.3122002395131601</v>
       </c>
       <c r="L119" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O119" t="s">
         <v>22</v>
       </c>
       <c r="P119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R119" t="s">
         <v>22</v>
       </c>
       <c r="S119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U119" t="s">
         <v>22</v>
       </c>
       <c r="V119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X119" t="s">
         <v>22</v>
       </c>
       <c r="Y119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA119" t="s">
         <v>22</v>
       </c>
       <c r="AB119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD119" t="s">
         <v>22</v>
       </c>
       <c r="AE119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG119" t="s">
         <v>22</v>
       </c>
       <c r="AH119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="120" spans="1:34">
@@ -3361,8 +3373,8 @@
       <c r="E120">
         <v>1.41</v>
       </c>
-      <c r="G120" s="1">
-        <v>-0.0004932280635475027</v>
+      <c r="G120" t="s">
+        <v>33</v>
       </c>
       <c r="I120">
         <v>7</v>
@@ -3371,7 +3383,7 @@
         <v>0.2687152090106903</v>
       </c>
       <c r="L120" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M120" s="2">
         <f>AVERAGE(P120:P126)</f>
@@ -3436,6 +3448,9 @@
       <c r="E121">
         <v>-0.17</v>
       </c>
+      <c r="G121" s="1">
+        <v>0.000493228063547533</v>
+      </c>
       <c r="I121">
         <v>8</v>
       </c>
@@ -3443,7 +3458,7 @@
         <v>0.2043964750703584</v>
       </c>
       <c r="L121" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M121" s="2">
         <f>AVERAGE(S120:S126)</f>
@@ -3508,6 +3523,9 @@
       <c r="E122">
         <v>0.62</v>
       </c>
+      <c r="G122" t="s">
+        <v>34</v>
+      </c>
       <c r="I122">
         <v>9</v>
       </c>
@@ -3515,7 +3533,7 @@
         <v>0.2228362332787754</v>
       </c>
       <c r="L122" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M122" s="2">
         <f>AVERAGE(V120:V126)</f>
@@ -3580,6 +3598,9 @@
       <c r="E123">
         <v>-0.48</v>
       </c>
+      <c r="G123" s="1">
+        <v>0.1642376570151589</v>
+      </c>
       <c r="I123">
         <v>10</v>
       </c>
@@ -3587,7 +3608,7 @@
         <v>0.1876723374506583</v>
       </c>
       <c r="L123" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M123" s="2">
         <f>AVERAGE(Y120:Y126)</f>
@@ -3659,7 +3680,7 @@
         <v>0.189224852533422</v>
       </c>
       <c r="L124" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M124" s="2">
         <f>AVERAGE(AB120:AB126)</f>
@@ -3731,7 +3752,7 @@
         <v>0.1970736318444489</v>
       </c>
       <c r="L125" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M125" s="2">
         <f>AVERAGE(AE120:AE126)</f>
@@ -3797,14 +3818,14 @@
         <v>-0.2</v>
       </c>
       <c r="I126" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J126" s="1">
         <f>AVERAGE(J119:J125)</f>
         <v>0</v>
       </c>
       <c r="L126" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M126" s="2">
         <f>AVERAGE(AH120:AH126)</f>
@@ -4467,7 +4488,7 @@
     </row>
     <row r="164" spans="1:34">
       <c r="A164" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="165" spans="1:34">
@@ -4478,10 +4499,10 @@
         <v>32</v>
       </c>
       <c r="I165" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L165" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="166" spans="1:34">
@@ -4507,31 +4528,31 @@
         <v>22</v>
       </c>
       <c r="J166" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L166" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O166" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R166" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U166" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X166" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA166" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD166" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG166" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="167" spans="1:34">
@@ -4550,9 +4571,6 @@
       <c r="E167">
         <v>-0.34</v>
       </c>
-      <c r="G167" t="s">
-        <v>33</v>
-      </c>
       <c r="I167">
         <v>6</v>
       </c>
@@ -4560,52 +4578,52 @@
         <v>0.2939463278814591</v>
       </c>
       <c r="L167" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O167" t="s">
         <v>22</v>
       </c>
       <c r="P167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R167" t="s">
         <v>22</v>
       </c>
       <c r="S167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U167" t="s">
         <v>22</v>
       </c>
       <c r="V167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X167" t="s">
         <v>22</v>
       </c>
       <c r="Y167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA167" t="s">
         <v>22</v>
       </c>
       <c r="AB167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD167" t="s">
         <v>22</v>
       </c>
       <c r="AE167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG167" t="s">
         <v>22</v>
       </c>
       <c r="AH167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="168" spans="1:34">
@@ -4624,8 +4642,8 @@
       <c r="E168">
         <v>0.34</v>
       </c>
-      <c r="G168" s="1">
-        <v>-0.006698279930065554</v>
+      <c r="G168" t="s">
+        <v>33</v>
       </c>
       <c r="I168">
         <v>7</v>
@@ -4634,7 +4652,7 @@
         <v>0.2617004335199791</v>
       </c>
       <c r="L168" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M168" s="2">
         <f>AVERAGE(P168:P174)</f>
@@ -4699,6 +4717,9 @@
       <c r="E169">
         <v>-1.63</v>
       </c>
+      <c r="G169" s="1">
+        <v>0.006698279930065534</v>
+      </c>
       <c r="I169">
         <v>8</v>
       </c>
@@ -4706,7 +4727,7 @@
         <v>0.1969648464605306</v>
       </c>
       <c r="L169" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M169" s="2">
         <f>AVERAGE(S168:S174)</f>
@@ -4771,6 +4792,9 @@
       <c r="E170">
         <v>-0.11</v>
       </c>
+      <c r="G170" t="s">
+        <v>34</v>
+      </c>
       <c r="I170">
         <v>9</v>
       </c>
@@ -4778,7 +4802,7 @@
         <v>0.1915081478496458</v>
       </c>
       <c r="L170" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M170" s="2">
         <f>AVERAGE(V168:V174)</f>
@@ -4843,6 +4867,9 @@
       <c r="E171">
         <v>-0.43</v>
       </c>
+      <c r="G171" s="1">
+        <v>0.2474545092571577</v>
+      </c>
       <c r="I171">
         <v>10</v>
       </c>
@@ -4850,7 +4877,7 @@
         <v>0.1761857678192239</v>
       </c>
       <c r="L171" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M171" s="2">
         <f>AVERAGE(Y168:Y174)</f>
@@ -4922,7 +4949,7 @@
         <v>0.1897269975916926</v>
       </c>
       <c r="L172" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M172" s="2">
         <f>AVERAGE(AB168:AB174)</f>
@@ -4994,7 +5021,7 @@
         <v>0.1601729845836288</v>
       </c>
       <c r="L173" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M173" s="2">
         <f>AVERAGE(AE168:AE174)</f>
@@ -5060,14 +5087,14 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="I174" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J174" s="1">
         <f>AVERAGE(J167:J173)</f>
         <v>0</v>
       </c>
       <c r="L174" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M174" s="2">
         <f>AVERAGE(AH168:AH174)</f>

</xml_diff>

<commit_message>
21.06.21 test_IntactFinder.py (just for RNA!!) 3
</commit_message>
<xml_diff>
--- a/Spectral_data/intact/x.xlsx
+++ b/Spectral_data/intact/x.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="52">
   <si>
     <t>parameters:</t>
   </si>
@@ -28,7 +28,7 @@
     <t>date:</t>
   </si>
   <si>
-    <t>21/06/2021 15:45</t>
+    <t>21/06/2021 16:15</t>
   </si>
   <si>
     <t>sequName</t>
@@ -115,10 +115,13 @@
     <t>av.charge:</t>
   </si>
   <si>
+    <t>calibration:</t>
+  </si>
+  <si>
     <t>av.error:</t>
   </si>
   <si>
-    <t>stddev.errors:</t>
+    <t>stddev.:</t>
   </si>
   <si>
     <t>av. number of modifications:</t>
@@ -624,10 +627,10 @@
         <v>32</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -653,31 +656,31 @@
         <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:34">
@@ -703,52 +706,52 @@
         <v>0.2883430282059997</v>
       </c>
       <c r="L19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O19" t="s">
         <v>22</v>
       </c>
       <c r="P19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R19" t="s">
         <v>22</v>
       </c>
       <c r="S19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U19" t="s">
         <v>22</v>
       </c>
       <c r="V19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X19" t="s">
         <v>22</v>
       </c>
       <c r="Y19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA19" t="s">
         <v>22</v>
       </c>
       <c r="AB19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD19" t="s">
         <v>22</v>
       </c>
       <c r="AE19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG19" t="s">
         <v>22</v>
       </c>
       <c r="AH19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:34">
@@ -777,7 +780,7 @@
         <v>0.2420044778973674</v>
       </c>
       <c r="L20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M20" s="2">
         <f>AVERAGE(P20:P26)</f>
@@ -842,7 +845,10 @@
       <c r="E21">
         <v>0.2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.001682549762607045</v>
       </c>
       <c r="I21">
@@ -852,7 +858,7 @@
         <v>0.2160532866805435</v>
       </c>
       <c r="L21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M21" s="2">
         <f>AVERAGE(S20:S26)</f>
@@ -918,7 +924,10 @@
         <v>0.8</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.1248090398552634</v>
       </c>
       <c r="I22">
         <v>9</v>
@@ -927,7 +936,7 @@
         <v>0.2142429496101891</v>
       </c>
       <c r="L22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M22" s="2">
         <f>AVERAGE(V20:V26)</f>
@@ -992,9 +1001,6 @@
       <c r="E23">
         <v>0.07000000000000001</v>
       </c>
-      <c r="G23" s="1">
-        <v>0.1248090398552634</v>
-      </c>
       <c r="I23">
         <v>10</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>0.1969289057698468</v>
       </c>
       <c r="L23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M23" s="2">
         <f>AVERAGE(Y20:Y26)</f>
@@ -1074,7 +1080,7 @@
         <v>0.1927280330419686</v>
       </c>
       <c r="L24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M24" s="2">
         <f>AVERAGE(AB20:AB26)</f>
@@ -1146,7 +1152,7 @@
         <v>0.1480257833164781</v>
       </c>
       <c r="L25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M25" s="2">
         <f>AVERAGE(AE20:AE26)</f>
@@ -1212,14 +1218,14 @@
         <v>0.11</v>
       </c>
       <c r="I26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J26" s="1">
         <f>AVERAGE(J19:J25)</f>
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M26" s="2">
         <f>AVERAGE(AH20:AH26)</f>
@@ -1916,7 +1922,7 @@
     </row>
     <row r="66" spans="1:34">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:34">
@@ -1927,10 +1933,10 @@
         <v>32</v>
       </c>
       <c r="I67" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:34">
@@ -1956,31 +1962,31 @@
         <v>22</v>
       </c>
       <c r="J68" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L68" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X68" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA68" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD68" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG68" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:34">
@@ -2006,52 +2012,52 @@
         <v>0.3058467421416752</v>
       </c>
       <c r="L69" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O69" t="s">
         <v>22</v>
       </c>
       <c r="P69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R69" t="s">
         <v>22</v>
       </c>
       <c r="S69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U69" t="s">
         <v>22</v>
       </c>
       <c r="V69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X69" t="s">
         <v>22</v>
       </c>
       <c r="Y69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA69" t="s">
         <v>22</v>
       </c>
       <c r="AB69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD69" t="s">
         <v>22</v>
       </c>
       <c r="AE69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG69" t="s">
         <v>22</v>
       </c>
       <c r="AH69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:34">
@@ -2080,7 +2086,7 @@
         <v>0.244000017611878</v>
       </c>
       <c r="L70" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M70" s="2">
         <f>AVERAGE(P70:P76)</f>
@@ -2145,7 +2151,10 @@
       <c r="E71">
         <v>1.54</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G71" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="1">
         <v>0.01632552560005641</v>
       </c>
       <c r="I71">
@@ -2155,7 +2164,7 @@
         <v>0.2214039362926656</v>
       </c>
       <c r="L71" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M71" s="2">
         <f>AVERAGE(S70:S76)</f>
@@ -2221,7 +2230,10 @@
         <v>0.64</v>
       </c>
       <c r="G72" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0.1823410545090352</v>
       </c>
       <c r="I72">
         <v>9</v>
@@ -2230,7 +2242,7 @@
         <v>0.1925425061385875</v>
       </c>
       <c r="L72" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M72" s="2">
         <f>AVERAGE(V70:V76)</f>
@@ -2295,9 +2307,6 @@
       <c r="E73">
         <v>-0.22</v>
       </c>
-      <c r="G73" s="1">
-        <v>0.1823410545090352</v>
-      </c>
       <c r="I73">
         <v>10</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>0.1855150789162632</v>
       </c>
       <c r="L73" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M73" s="2">
         <f>AVERAGE(Y70:Y76)</f>
@@ -2377,7 +2386,7 @@
         <v>0.193393580483101</v>
       </c>
       <c r="L74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M74" s="2">
         <f>AVERAGE(AB70:AB76)</f>
@@ -2449,7 +2458,7 @@
         <v>0.166940412656703</v>
       </c>
       <c r="L75" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M75" s="2">
         <f>AVERAGE(AE70:AE76)</f>
@@ -2515,14 +2524,14 @@
         <v>0.34</v>
       </c>
       <c r="I76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J76" s="1">
         <f>AVERAGE(J69:J75)</f>
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M76" s="2">
         <f>AVERAGE(AH70:AH76)</f>
@@ -3219,7 +3228,7 @@
     </row>
     <row r="116" spans="1:34">
       <c r="A116" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="117" spans="1:34">
@@ -3230,10 +3239,10 @@
         <v>32</v>
       </c>
       <c r="I117" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L117" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="118" spans="1:34">
@@ -3259,31 +3268,31 @@
         <v>22</v>
       </c>
       <c r="J118" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L118" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O118" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R118" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U118" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X118" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA118" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD118" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG118" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="119" spans="1:34">
@@ -3309,52 +3318,52 @@
         <v>0.3122002395131601</v>
       </c>
       <c r="L119" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O119" t="s">
         <v>22</v>
       </c>
       <c r="P119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R119" t="s">
         <v>22</v>
       </c>
       <c r="S119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U119" t="s">
         <v>22</v>
       </c>
       <c r="V119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X119" t="s">
         <v>22</v>
       </c>
       <c r="Y119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA119" t="s">
         <v>22</v>
       </c>
       <c r="AB119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD119" t="s">
         <v>22</v>
       </c>
       <c r="AE119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG119" t="s">
         <v>22</v>
       </c>
       <c r="AH119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:34">
@@ -3383,7 +3392,7 @@
         <v>0.2687152090106903</v>
       </c>
       <c r="L120" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M120" s="2">
         <f>AVERAGE(P120:P126)</f>
@@ -3448,7 +3457,10 @@
       <c r="E121">
         <v>-0.17</v>
       </c>
-      <c r="G121" s="1">
+      <c r="G121" t="s">
+        <v>34</v>
+      </c>
+      <c r="H121" s="1">
         <v>0.000493228063547533</v>
       </c>
       <c r="I121">
@@ -3458,7 +3470,7 @@
         <v>0.2043964750703584</v>
       </c>
       <c r="L121" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M121" s="2">
         <f>AVERAGE(S120:S126)</f>
@@ -3524,7 +3536,10 @@
         <v>0.62</v>
       </c>
       <c r="G122" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0.1642376570151589</v>
       </c>
       <c r="I122">
         <v>9</v>
@@ -3533,7 +3548,7 @@
         <v>0.2228362332787754</v>
       </c>
       <c r="L122" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M122" s="2">
         <f>AVERAGE(V120:V126)</f>
@@ -3598,9 +3613,6 @@
       <c r="E123">
         <v>-0.48</v>
       </c>
-      <c r="G123" s="1">
-        <v>0.1642376570151589</v>
-      </c>
       <c r="I123">
         <v>10</v>
       </c>
@@ -3608,7 +3620,7 @@
         <v>0.1876723374506583</v>
       </c>
       <c r="L123" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M123" s="2">
         <f>AVERAGE(Y120:Y126)</f>
@@ -3680,7 +3692,7 @@
         <v>0.189224852533422</v>
       </c>
       <c r="L124" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M124" s="2">
         <f>AVERAGE(AB120:AB126)</f>
@@ -3752,7 +3764,7 @@
         <v>0.1970736318444489</v>
       </c>
       <c r="L125" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M125" s="2">
         <f>AVERAGE(AE120:AE126)</f>
@@ -3818,14 +3830,14 @@
         <v>-0.2</v>
       </c>
       <c r="I126" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J126" s="1">
         <f>AVERAGE(J119:J125)</f>
         <v>0</v>
       </c>
       <c r="L126" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M126" s="2">
         <f>AVERAGE(AH120:AH126)</f>
@@ -4488,7 +4500,7 @@
     </row>
     <row r="164" spans="1:34">
       <c r="A164" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="165" spans="1:34">
@@ -4499,10 +4511,10 @@
         <v>32</v>
       </c>
       <c r="I165" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L165" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="166" spans="1:34">
@@ -4528,31 +4540,31 @@
         <v>22</v>
       </c>
       <c r="J166" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L166" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O166" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R166" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U166" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X166" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA166" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD166" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG166" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="167" spans="1:34">
@@ -4578,52 +4590,52 @@
         <v>0.2939463278814591</v>
       </c>
       <c r="L167" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O167" t="s">
         <v>22</v>
       </c>
       <c r="P167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R167" t="s">
         <v>22</v>
       </c>
       <c r="S167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U167" t="s">
         <v>22</v>
       </c>
       <c r="V167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X167" t="s">
         <v>22</v>
       </c>
       <c r="Y167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA167" t="s">
         <v>22</v>
       </c>
       <c r="AB167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD167" t="s">
         <v>22</v>
       </c>
       <c r="AE167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG167" t="s">
         <v>22</v>
       </c>
       <c r="AH167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" spans="1:34">
@@ -4652,7 +4664,7 @@
         <v>0.2617004335199791</v>
       </c>
       <c r="L168" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M168" s="2">
         <f>AVERAGE(P168:P174)</f>
@@ -4717,7 +4729,10 @@
       <c r="E169">
         <v>-1.63</v>
       </c>
-      <c r="G169" s="1">
+      <c r="G169" t="s">
+        <v>34</v>
+      </c>
+      <c r="H169" s="1">
         <v>0.006698279930065534</v>
       </c>
       <c r="I169">
@@ -4727,7 +4742,7 @@
         <v>0.1969648464605306</v>
       </c>
       <c r="L169" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M169" s="2">
         <f>AVERAGE(S168:S174)</f>
@@ -4793,7 +4808,10 @@
         <v>-0.11</v>
       </c>
       <c r="G170" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="H170" s="1">
+        <v>0.2474545092571577</v>
       </c>
       <c r="I170">
         <v>9</v>
@@ -4802,7 +4820,7 @@
         <v>0.1915081478496458</v>
       </c>
       <c r="L170" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M170" s="2">
         <f>AVERAGE(V168:V174)</f>
@@ -4867,9 +4885,6 @@
       <c r="E171">
         <v>-0.43</v>
       </c>
-      <c r="G171" s="1">
-        <v>0.2474545092571577</v>
-      </c>
       <c r="I171">
         <v>10</v>
       </c>
@@ -4877,7 +4892,7 @@
         <v>0.1761857678192239</v>
       </c>
       <c r="L171" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M171" s="2">
         <f>AVERAGE(Y168:Y174)</f>
@@ -4949,7 +4964,7 @@
         <v>0.1897269975916926</v>
       </c>
       <c r="L172" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M172" s="2">
         <f>AVERAGE(AB168:AB174)</f>
@@ -5021,7 +5036,7 @@
         <v>0.1601729845836288</v>
       </c>
       <c r="L173" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M173" s="2">
         <f>AVERAGE(AE168:AE174)</f>
@@ -5087,14 +5102,14 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="I174" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J174" s="1">
         <f>AVERAGE(J167:J173)</f>
         <v>0</v>
       </c>
       <c r="L174" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M174" s="2">
         <f>AVERAGE(AH168:AH174)</f>

</xml_diff>